<commit_message>
Refactor work order record steps to use new action classes for improved organization and maintainability
- Updated imports to use new action classes for task checklists, work order records, and related functionalities.
- Replaced direct page interactions with action methods in the following step files:
  - task.checklists.steps.ts
  - cancel.wko.steps.ts
  - close.wko.steps.ts
  - create.layout.step.ts
  - delete.wko.steps.ts
  - hold.wko.steps.ts
  - label.change.steps.ts
  - listview.search.filters.steps.ts
  - omit.lookup.wko.steps.ts
  - search.update.wko.steps.ts
  - sorting.wko.steps.ts
- Enhanced code readability and maintainability by consolidating page interactions into dedicated action classes.
</commit_message>
<xml_diff>
--- a/src/data/testData/MPulse.xlsx
+++ b/src/data/testData/MPulse.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MPulse\src\data\testData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C0368F0-BD8E-4F8F-91C0-AACD04DE06FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11160"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login_Page" sheetId="1" r:id="rId1"/>
@@ -14,32 +20,29 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>USERNAME</t>
   </si>
   <si>
     <t>shrikant@inapp.com</t>
   </si>
+  <si>
+    <t>PASSWORD</t>
+  </si>
+  <si>
+    <t/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,10 +95,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -103,7 +107,7 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Invisible" pivot="0" table="0" count="0"/>
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}"/>
   </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -405,18 +409,18 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -425,19 +429,25 @@
     <col min="2" max="2" width="27.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="2" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>